<commit_message>
changes in libs and templates
</commit_message>
<xml_diff>
--- a/CapGOST.xlsx
+++ b/CapGOST.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DDF430-6C27-40E5-A235-DF92AB0FCF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB9399B-B701-4C3B-8439-CAD87C71DB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="139">
   <si>
     <t>Part Number</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>CAP15x13x1</t>
+  </si>
+  <si>
+    <t>GRM32ER71H475KA88L</t>
+  </si>
+  <si>
+    <t>4,7мкФ</t>
   </si>
 </sst>
 </file>
@@ -953,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2193,7 @@
         <v xml:space="preserve">К53-65 "E"-50В-10мкФ±10% АЖЯР.673546.004ТУ </v>
       </c>
       <c r="M28" s="5" t="str">
-        <f t="shared" ref="M28:M40" si="3">G28</f>
+        <f t="shared" ref="M28:M41" si="3">G28</f>
         <v>10мкФ</v>
       </c>
     </row>
@@ -2595,6 +2601,33 @@
       <c r="M40" s="5" t="str">
         <f t="shared" si="3"/>
         <v>12пФ</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="M41" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>4,7мкФ</v>
       </c>
     </row>
   </sheetData>

</xml_diff>